<commit_message>
fix: changes to gastro report template document
</commit_message>
<xml_diff>
--- a/Aplikácia/tools/gastro-report-template.xlsx
+++ b/Aplikácia/tools/gastro-report-template.xlsx
@@ -11,9 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
-  <si>
-    <t>107420-KAI</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+  <si>
+    <t>{departmentId}</t>
   </si>
   <si>
     <t>Por. číslo</t>
@@ -40,7 +40,40 @@
     <t>Poznámka pre MU</t>
   </si>
   <si>
+    <t>Obdobie: {month_sk} {year}</t>
+  </si>
+  <si>
+    <t>{i + 1}</t>
+  </si>
+  <si>
+    <t>{personal_id}</t>
+  </si>
+  <si>
+    <t>{surname}</t>
+  </si>
+  <si>
+    <t>{name}</t>
+  </si>
+  <si>
+    <t>{budget}</t>
+  </si>
+  <si>
+    <t>{sub}</t>
+  </si>
+  <si>
+    <t>{diff}</t>
+  </si>
+  <si>
+    <t>{note}</t>
+  </si>
+  <si>
     <t>CELKOM</t>
+  </si>
+  <si>
+    <t>{narok}</t>
+  </si>
+  <si>
+    <t>{zaloha}</t>
   </si>
 </sst>
 </file>
@@ -153,7 +186,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -172,9 +205,6 @@
     <xf numFmtId="49" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -184,17 +214,17 @@
     <xf numFmtId="1" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -206,9 +236,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -223,8 +250,8 @@
     <xf numFmtId="2" fontId="2" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -1281,7 +1308,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
@@ -1290,13 +1317,13 @@
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="8.75781" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.8125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1719" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.8125" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.8594" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.42969" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.1719" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42188" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85156" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6719" style="1" customWidth="1"/>
     <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1316,75 +1343,108 @@
       <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="6">
+      <c r="E2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="6">
+      <c r="F2" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="7">
+      <c r="G2" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="8">
+      <c r="H2" t="s" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="3" ht="22.7" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+    <row r="3" ht="40.9" customHeight="1">
+      <c r="A3" s="8"/>
+      <c r="B3" t="s" s="5">
+        <v>9</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" ht="22.7" customHeight="1">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="17"/>
+      <c r="A4" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s" s="11">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s" s="12">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" ht="22.7" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" ht="22.7" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" t="s" s="20">
-        <v>9</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="24"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" ht="22.7" customHeight="1">
+      <c r="A7" s="17"/>
+      <c r="B7" t="s" s="18">
+        <v>18</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" t="s" s="18">
+        <v>19</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" t="s" s="21">
+        <v>20</v>
+      </c>
+      <c r="H7" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B3:G3"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
fix: add data types to cells
</commit_message>
<xml_diff>
--- a/Aplikácia/tools/gastro-report-template.xlsx
+++ b/Aplikácia/tools/gastro-report-template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>{departmentId}</t>
   </si>
@@ -41,30 +41,6 @@
   </si>
   <si>
     <t>Obdobie: {month_sk} {year}</t>
-  </si>
-  <si>
-    <t>{i + 1}</t>
-  </si>
-  <si>
-    <t>{personal_id}</t>
-  </si>
-  <si>
-    <t>{surname}</t>
-  </si>
-  <si>
-    <t>{name}</t>
-  </si>
-  <si>
-    <t>{budget}</t>
-  </si>
-  <si>
-    <t>{sub}</t>
-  </si>
-  <si>
-    <t>{diff}</t>
-  </si>
-  <si>
-    <t>{note}</t>
   </si>
   <si>
     <t>CELKOM</t>
@@ -186,7 +162,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -220,7 +196,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1378,40 +1363,24 @@
       <c r="H3" s="10"/>
     </row>
     <row r="4" ht="22.7" customHeight="1">
-      <c r="A4" t="s" s="11">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s" s="5">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s" s="11">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s" s="6">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s" s="12">
-        <v>17</v>
-      </c>
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" ht="22.7" customHeight="1">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="16"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" ht="22.7" customHeight="1">
       <c r="A6" s="8"/>
@@ -1424,20 +1393,20 @@
       <c r="H6" s="9"/>
     </row>
     <row r="7" ht="22.7" customHeight="1">
-      <c r="A7" s="17"/>
-      <c r="B7" t="s" s="18">
-        <v>18</v>
+      <c r="A7" s="20"/>
+      <c r="B7" t="s" s="21">
+        <v>10</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" t="s" s="18">
-        <v>19</v>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" t="s" s="21">
+        <v>11</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" t="s" s="21">
-        <v>20</v>
+      <c r="F7" s="23"/>
+      <c r="G7" t="s" s="24">
+        <v>12</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>